<commit_message>
update IBES; construct UCONS for 10-Q
</commit_message>
<xml_diff>
--- a/output/UT_6.xlsx
+++ b/output/UT_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\narrative_conservatism\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CC26844A-0FBD-4C5F-9968-525A00C1DC42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC316F55-5E82-4DEB-A2A1-82FD5EF69F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="124">
   <si>
     <t/>
   </si>
@@ -34,6 +34,27 @@
     <t>(3)</t>
   </si>
   <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(7)</t>
+  </si>
+  <si>
+    <t>(8)</t>
+  </si>
+  <si>
+    <t>(9)</t>
+  </si>
+  <si>
+    <t>VARIABLES</t>
+  </si>
+  <si>
     <t>NW</t>
   </si>
   <si>
@@ -43,223 +64,277 @@
     <t>TLAG</t>
   </si>
   <si>
-    <t>0.256***</t>
-  </si>
-  <si>
-    <t>(22.66)</t>
-  </si>
-  <si>
-    <t>-0.174***</t>
-  </si>
-  <si>
-    <t>-0.320***</t>
-  </si>
-  <si>
-    <t>-2.812***</t>
-  </si>
-  <si>
-    <t>(-3.27)</t>
-  </si>
-  <si>
-    <t>(-7.26)</t>
-  </si>
-  <si>
-    <t>(-4.21)</t>
-  </si>
-  <si>
-    <t>-0.019***</t>
-  </si>
-  <si>
-    <t>(-3.23)</t>
-  </si>
-  <si>
-    <t>0.648***</t>
-  </si>
-  <si>
-    <t>(91.90)</t>
-  </si>
-  <si>
-    <t>-0.012**</t>
-  </si>
-  <si>
-    <t>(-2.46)</t>
-  </si>
-  <si>
-    <t>0.022</t>
-  </si>
-  <si>
-    <t>(1.31)</t>
-  </si>
-  <si>
-    <t>0.076***</t>
-  </si>
-  <si>
-    <t>(4.33)</t>
-  </si>
-  <si>
-    <t>0.215***</t>
-  </si>
-  <si>
-    <t>(22.82)</t>
-  </si>
-  <si>
-    <t>-0.069</t>
-  </si>
-  <si>
-    <t>-0.420***</t>
-  </si>
-  <si>
-    <t>-0.055</t>
-  </si>
-  <si>
-    <t>(-1.54)</t>
-  </si>
-  <si>
-    <t>(-9.29)</t>
-  </si>
-  <si>
-    <t>(-0.14)</t>
-  </si>
-  <si>
-    <t>-0.007</t>
-  </si>
-  <si>
-    <t>(-1.40)</t>
-  </si>
-  <si>
-    <t>0.520***</t>
-  </si>
-  <si>
-    <t>(62.06)</t>
-  </si>
-  <si>
-    <t>-0.009**</t>
-  </si>
-  <si>
-    <t>(-2.10)</t>
-  </si>
-  <si>
-    <t>0.057***</t>
-  </si>
-  <si>
-    <t>(5.54)</t>
-  </si>
-  <si>
-    <t>0.004</t>
-  </si>
-  <si>
-    <t>(0.37)</t>
-  </si>
-  <si>
-    <t>0.248***</t>
-  </si>
-  <si>
-    <t>(29.03)</t>
-  </si>
-  <si>
-    <t>-0.115**</t>
-  </si>
-  <si>
-    <t>-0.436***</t>
-  </si>
-  <si>
-    <t>1.278***</t>
-  </si>
-  <si>
-    <t>(-2.40)</t>
-  </si>
-  <si>
-    <t>(-8.99)</t>
-  </si>
-  <si>
-    <t>(3.11)</t>
-  </si>
-  <si>
-    <t>-0.011**</t>
-  </si>
-  <si>
-    <t>(-2.17)</t>
-  </si>
-  <si>
-    <t>0.443***</t>
-  </si>
-  <si>
-    <t>(49.27)</t>
-  </si>
-  <si>
-    <t>-0.010**</t>
-  </si>
-  <si>
-    <t>(-2.32)</t>
-  </si>
-  <si>
-    <t>0.044***</t>
-  </si>
-  <si>
-    <t>(6.40)</t>
-  </si>
-  <si>
-    <t>-0.030***</t>
-  </si>
-  <si>
-    <t>(-2.86)</t>
+    <t>LAG1_NW</t>
+  </si>
+  <si>
+    <t>0.253***</t>
+  </si>
+  <si>
+    <t>(21.27)</t>
+  </si>
+  <si>
+    <t>NEG</t>
+  </si>
+  <si>
+    <t>-0.125***</t>
+  </si>
+  <si>
+    <t>-0.365***</t>
+  </si>
+  <si>
+    <t>2.329***</t>
+  </si>
+  <si>
+    <t>-0.144***</t>
+  </si>
+  <si>
+    <t>-0.486***</t>
+  </si>
+  <si>
+    <t>0.884**</t>
+  </si>
+  <si>
+    <t>-0.126**</t>
+  </si>
+  <si>
+    <t>-0.504***</t>
+  </si>
+  <si>
+    <t>1.145***</t>
+  </si>
+  <si>
+    <t>(-2.66)</t>
+  </si>
+  <si>
+    <t>(-9.31)</t>
+  </si>
+  <si>
+    <t>(2.66)</t>
+  </si>
+  <si>
+    <t>(-3.07)</t>
+  </si>
+  <si>
+    <t>(-11.89)</t>
+  </si>
+  <si>
+    <t>(2.42)</t>
+  </si>
+  <si>
+    <t>(-2.43)</t>
+  </si>
+  <si>
+    <t>(-11.73)</t>
+  </si>
+  <si>
+    <t>(2.71)</t>
+  </si>
+  <si>
+    <t>LAG1_NW_NEG</t>
+  </si>
+  <si>
+    <t>-0.013**</t>
+  </si>
+  <si>
+    <t>(-2.56)</t>
+  </si>
+  <si>
+    <t>LAG1_TONE</t>
+  </si>
+  <si>
+    <t>0.650***</t>
+  </si>
+  <si>
+    <t>(95.16)</t>
+  </si>
+  <si>
+    <t>LAG1_TONE_NEG</t>
+  </si>
+  <si>
+    <t>-0.014***</t>
+  </si>
+  <si>
+    <t>(-3.74)</t>
+  </si>
+  <si>
+    <t>LAG1_TLAG</t>
+  </si>
+  <si>
+    <t>0.077***</t>
+  </si>
+  <si>
+    <t>(4.40)</t>
+  </si>
+  <si>
+    <t>LAG1_TLAG_NEG</t>
+  </si>
+  <si>
+    <t>-0.056**</t>
+  </si>
+  <si>
+    <t>(-2.44)</t>
+  </si>
+  <si>
+    <t>LAG2_NW</t>
+  </si>
+  <si>
+    <t>0.219***</t>
+  </si>
+  <si>
+    <t>(24.08)</t>
+  </si>
+  <si>
+    <t>LAG2_NW_NEG</t>
+  </si>
+  <si>
+    <t>-0.015***</t>
+  </si>
+  <si>
+    <t>(-2.91)</t>
+  </si>
+  <si>
+    <t>LAG2_TONE</t>
+  </si>
+  <si>
+    <t>0.525***</t>
+  </si>
+  <si>
+    <t>(63.88)</t>
+  </si>
+  <si>
+    <t>LAG2_TONE_NEG</t>
+  </si>
+  <si>
+    <t>-0.018***</t>
+  </si>
+  <si>
+    <t>(-4.49)</t>
+  </si>
+  <si>
+    <t>LAG2_TLAG</t>
+  </si>
+  <si>
+    <t>0.070***</t>
+  </si>
+  <si>
+    <t>(9.73)</t>
+  </si>
+  <si>
+    <t>LAG2_TLAG_NEG</t>
+  </si>
+  <si>
+    <t>-0.018*</t>
+  </si>
+  <si>
+    <t>(-1.91)</t>
+  </si>
+  <si>
+    <t>LAG3_NW</t>
+  </si>
+  <si>
+    <t>0.249***</t>
+  </si>
+  <si>
+    <t>(29.44)</t>
+  </si>
+  <si>
+    <t>LAG3_NW_NEG</t>
+  </si>
+  <si>
+    <t>(-2.27)</t>
+  </si>
+  <si>
+    <t>LAG3_TONE</t>
+  </si>
+  <si>
+    <t>0.449***</t>
+  </si>
+  <si>
+    <t>(49.00)</t>
+  </si>
+  <si>
+    <t>LAG3_TONE_NEG</t>
+  </si>
+  <si>
+    <t>-0.021***</t>
+  </si>
+  <si>
+    <t>(-4.44)</t>
+  </si>
+  <si>
+    <t>LAG3_TLAG</t>
+  </si>
+  <si>
+    <t>0.039***</t>
+  </si>
+  <si>
+    <t>(6.33)</t>
+  </si>
+  <si>
+    <t>LAG3_TLAG_NEG</t>
+  </si>
+  <si>
+    <t>-0.025**</t>
+  </si>
+  <si>
+    <t>(-2.29)</t>
   </si>
   <si>
     <t>Constant</t>
   </si>
   <si>
-    <t>-6.326***</t>
-  </si>
-  <si>
-    <t>-2.644***</t>
-  </si>
-  <si>
-    <t>39.409***</t>
-  </si>
-  <si>
-    <t>-5.911***</t>
-  </si>
-  <si>
-    <t>4.677***</t>
-  </si>
-  <si>
-    <t>30.728***</t>
-  </si>
-  <si>
-    <t>-5.797***</t>
-  </si>
-  <si>
-    <t>-1.444</t>
-  </si>
-  <si>
-    <t>41.567***</t>
-  </si>
-  <si>
-    <t>(-61.89)</t>
-  </si>
-  <si>
-    <t>(-12.50)</t>
-  </si>
-  <si>
-    <t>(52.17)</t>
-  </si>
-  <si>
-    <t>(-69.33)</t>
-  </si>
-  <si>
-    <t>(5.43)</t>
-  </si>
-  <si>
-    <t>(4.53)</t>
-  </si>
-  <si>
-    <t>(-58.19)</t>
-  </si>
-  <si>
-    <t>(-0.45)</t>
-  </si>
-  <si>
-    <t>(63.78)</t>
+    <t>-6.376***</t>
+  </si>
+  <si>
+    <t>-2.749***</t>
+  </si>
+  <si>
+    <t>37.490***</t>
+  </si>
+  <si>
+    <t>-5.860***</t>
+  </si>
+  <si>
+    <t>4.814***</t>
+  </si>
+  <si>
+    <t>31.860***</t>
+  </si>
+  <si>
+    <t>-5.781***</t>
+  </si>
+  <si>
+    <t>-1.140</t>
+  </si>
+  <si>
+    <t>41.596***</t>
+  </si>
+  <si>
+    <t>(-60.05)</t>
+  </si>
+  <si>
+    <t>(-13.09)</t>
+  </si>
+  <si>
+    <t>(45.16)</t>
+  </si>
+  <si>
+    <t>(-69.13)</t>
+  </si>
+  <si>
+    <t>(5.91)</t>
+  </si>
+  <si>
+    <t>(5.55)</t>
+  </si>
+  <si>
+    <t>(-53.51)</t>
+  </si>
+  <si>
+    <t>(-0.37)</t>
+  </si>
+  <si>
+    <t>(75.13)</t>
   </si>
   <si>
     <t>Observations</t>
@@ -283,15 +358,15 @@
     <t>0.764</t>
   </si>
   <si>
+    <t>0.636</t>
+  </si>
+  <si>
+    <t>0.707</t>
+  </si>
+  <si>
     <t>0.637</t>
   </si>
   <si>
-    <t>0.707</t>
-  </si>
-  <si>
-    <t>0.636</t>
-  </si>
-  <si>
     <t>0.726</t>
   </si>
   <si>
@@ -317,28 +392,13 @@
   </si>
   <si>
     <t>*** p&lt;0.01, ** p&lt;0.05, * p&lt;0.1</t>
-  </si>
-  <si>
-    <t>DEP</t>
-  </si>
-  <si>
-    <t>LAGN_DEP</t>
-  </si>
-  <si>
-    <t>LAGN_NEG</t>
-  </si>
-  <si>
-    <t>LAGN_DEP_LAGN_NEG</t>
-  </si>
-  <si>
-    <t>LAGN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -487,13 +547,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,12 +726,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -858,7 +907,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -873,17 +922,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1239,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A39" activeCellId="8" sqref="A5:XFD6 A11:XFD12 A15:XFD16 A19:XFD20 A23:XFD24 A27:XFD28 A31:XFD32 A35:XFD36 A39:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1252,55 +1290,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="A2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1337,34 +1387,34 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1372,63 +1422,63 @@
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1436,127 +1486,127 @@
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>59</v>
+      <c r="C9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>60</v>
+      <c r="C10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1564,42 +1614,42 @@
         <v>0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>0</v>
@@ -1625,181 +1675,1199 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="5" t="s">
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="7" t="s">
+      <c r="C44" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
+      <c r="D44" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="E44" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>